<commit_message>
modify prompt for classify
</commit_message>
<xml_diff>
--- a/evaluate/data/data_evaluate_Hanoi.xlsx
+++ b/evaluate/data/data_evaluate_Hanoi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDTU\Year_4_Semester1\Dự án\Code\evaluate\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C8C12A0-E77C-49A7-917E-A4EF423EBB79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D3CBDD-83B6-464F-817A-4BC1B095C052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Question</t>
   </si>
@@ -192,6 +192,409 @@
   </si>
   <si>
     <t>Amelié Homestay mang đến một không gian vừa gần gũi vừa tinh tế, chỉ cách Hồ Hoàn Kiếm và Nhà hát Múa rối Nước Thăng Long vài bước chân, giúp du khách dễ dàng tận hưởng nét đẹp phố cổ. Các phòng được thiết kế ấm cúng, có ánh sáng dịu, ban công nhỏ hướng phố để nhâm nhi trà và ngắm dòng người. Nội thất đơn giản nhưng đủ tiện nghi như wifi tốc độ cao, điều hòa, tủ lạnh mini, bàn trà. Du khách đánh giá cao sự sạch sẽ và giường êm ái, cùng với chủ nhà thân thiện, hỗ trợ nhanh. Đây là nơi thuận tiện, đẹp, giá hợp lý, phù hợp để cảm nhận nhịp sống Hà Nội.</t>
+  </si>
+  <si>
+    <t>Phong cách thiết kế và điểm nổi bật của Veque Homestay là gì?</t>
+  </si>
+  <si>
+    <t>Veque Homestay nằm ngay tại trung tâm phố cổ Hà Nội và được thiết kế lấy cảm hứng từ vùng quê Bắc Bộ thời xưa cũ. Khi đến với Veque Homestay, du khách sẽ dễ dàng bắt gặp các món đồ cổ độc đáo như tấm màn gió làm từ vải hoa, tranh thôn nữ, nền gạch hoa xưa cũ, đồ gốm sứ. Các gam màu trung tính được kết hợp hài hòa, khiến không gian homestay trở nên khác lạ. Từ đây du khách cũng dễ dàng di chuyển đến các điểm tham quan như chợ Đồng Xuân, hồ Hoàn Kiếm, phố cổ Hà Nội.</t>
+  </si>
+  <si>
+    <t>Điểm nổi bật nhất của The Moonlight – Homestay ở Sóc Sơn là gì?</t>
+  </si>
+  <si>
+    <t>The Moonlight – Homestay ở Sóc Sơn là một trong những homestay có góc view rất đắt giá, thu hút nhiều bạn trẻ bởi vẻ đẹp thiên nhiên và thơ mộng. Nơi đây có cảnh núi rừng xanh đẫm, mát mẻ, cùng chiếc cửa sổ mờ ảo trong làn sương buổi sáng sớm và tiếng chim hót vang cả một vùng trời. Hệ thống nhà của The Moonlight được xây dựng bằng kính, với kính trong suốt ở hầu hết các phòng để du khách có thể thoải mái ngắm nhìn khung cảnh nơi đây.</t>
+  </si>
+  <si>
+    <t>Lacaito Homestay Hà Nội nằm ở đâu và có đặc điểm gì nổi bật?</t>
+  </si>
+  <si>
+    <t>Lacaito Homestay Hà Nội nằm tại số 2 Dã Tượng, phường Trần Hưng Đạo, quận Hoàn Kiếm, thành phố Hà Nội, với giá tham khảo từ 500.000đ/đêm. Đây là một ngôi nhà nhỏ duyên dáng nằm trong con ngõ ở trung tâm Hà Nội nhưng tách biệt khỏi sự ồn ào. Homestay yên tĩnh, xinh xắn, trang trí dễ thương và góc nào chụp ảnh cũng đẹp. Vào những ngày lộng gió, ngồi ở Lacaito cùng tách cà phê và một cuốn sách sẽ mang lại cảm giác bình yên.</t>
+  </si>
+  <si>
+    <t>Tre House Hà Nội nằm ở đâu và homestay này có những điểm nổi bật gì?</t>
+  </si>
+  <si>
+    <t>Tre House nằm tại địa chỉ 781 Hồng Hà, Chương Dương Độ, quận Hoàn Kiếm, Hà Nội, với giá từ 500.000đ/đêm. Homestay có phong cách hoài cổ nhưng vẫn đầy đủ tiện nghi hiện đại, tạo cảm giác thân thiện, ấm áp và riêng tư cho khách. Chủ nhà sắp xếp từng phòng rất chỉn chu. Tre House có một rooftop trên cao dùng để ngắm cảnh đẹp, thưởng thức hoàng hôn, uống trà, đọc sách và gặp gỡ những vị khách khác.</t>
+  </si>
+  <si>
+    <t>Hãy mô tả toàn bộ đặc điểm của Carrot House Hà Nội, bao gồm địa chỉ, thiết kế, sức chứa, tiện nghi nổi bật và các hỗ trợ dành cho khách.</t>
+  </si>
+  <si>
+    <t>Carrot House nằm tại địa chỉ 2C ngõ Bảo Khánh, Hoàn Kiếm, Hà Nội. Homestay này nằm trên tầng 3 của một tòa nhà mang thiết kế kiểu Pháp từ những năm 1900. Phòng ngủ có cửa kính lớn tạo cảm giác thoáng mát và rộng hơn. Căn hộ có 1 phòng ngủ chính gồm giường cỡ Queen, 1 giường đơn và thêm 2 nệm, toilet khép kín. Ngoài ra còn có một phòng khách rộng rãi với giường và sofa, phù hợp phục vụ nhóm từ khoảng 8–12 người. Phía trước căn hộ có một ban công lớn, nơi khách có thể ngắm cảnh hoặc tổ chức tiệc nướng ngoài trời. Thời gian check-in là 14h và check-out là 12h. Chủ nhà có hỗ trợ đặt xe đưa đón tận sân bay và luôn sẵn sàng hỗ trợ khi khách cần.</t>
+  </si>
+  <si>
+    <t>Hãy mô tả chi tiết Nhà ven hồ – Ba Vì Homestay, bao gồm: địa chỉ, giá phòng, phong cách thiết kế và chất liệu chính, số lượng phòng ngủ, các tiện nghi trong mỗi phòng, không gian xung quanh, cùng toàn bộ các dịch vụ – hoạt động đi kèm như ăn uống, xe di chuyển nội khu, các loại bể bơi và BBQ ngoài trời.</t>
+  </si>
+  <si>
+    <t>Nhà ven hồ – Ba Vì Homestay có địa chỉ tại Đồng Mô, Ba Vì, Sơn Tây, Hà Nội, giá phòng 2.000.000đ. Đây là một trong những homestay gần Hà Nội thuộc nhóm ít homestay Ba Vì mang đến cho du khách cảm giác thư thái, nhẹ nhàng khi nghỉ dưỡng. Homestay được xây dựng trên một khu đất trống vô cùng rộng rãi, với lối thiết kế kiểu phương Tây nhưng vẫn mang đậm chất truyền thống nhờ cỏ cây hoa lá xung quanh.
+Hiện tại, Nhà ven hồ homestay có tổng cộng 6 phòng ngủ cho khách nghỉ dưỡng. Các phòng ngủ được thiết kế đơn giản theo phong cách truyền thống Việt Nam, sử dụng nhiều gỗ tự nhiên với tông màu trắng và nâu tạo cảm giác ấm áp. Mỗi phòng đều được trang bị đầy đủ tiện nghi và các thiết bị điện tử như tivi, đầu đĩa DVD, tủ lạnh và máy pha trà/cà phê. Các phòng còn có cửa sổ lớn để tận dụng tối đa ánh sáng tự nhiên và tầm nhìn ra khu vườn xung quanh. Trong phòng có thêm những chiếc ghế mây tre đan, khiến không gian vừa hiện đại vừa dân dã. Tất cả các phòng đều được bố trí nhằm mang lại sự thoải mái và thư giãn tối đa cho khách.
+Về dịch vụ đi kèm, Nhà ven hồ – Ba Vì Homestay cung cấp 1 bữa ăn sáng buffet tại nhà hàng tre Vedana, miễn phí trà, cà phê và hoa quả tiêu chuẩn tại phòng. Mỗi căn villa được miễn phí sử dụng 2 xe đạp, đồng thời có hỗ trợ xe điện di chuyển trong khuôn viên homestay. Khách được sử dụng bể bơi riêng tại từng căn villa và bể bơi vô cực ngoài trời tại khu trung tâm của Vedana. Nếu muốn sử dụng bể bơi nước khoáng nóng, khách cần mua vé với giá 200.000 VNĐ/người lớn. Đặc biệt, khi đến với Nhà ven hồ homestay, du khách có thể tận hưởng những bữa tiệc BBQ ngoài trời cùng bạn bè và người thân, với toàn bộ đồ dùng luôn được nhân viên chuẩn bị đầy đủ. Trong khuôn viên homestay còn có vườn rau, nơi khách có thể tự tay hái rau sạch tại vườn để bổ sung cho bữa tiệc BBQ tối mà không cần trả thêm khoản phí nào.</t>
+  </si>
+  <si>
+    <t>Trong số các homestay thuộc khu vực Sóc Sơn, nơi phù hợp nhất cho một cặp đôi muốn nghỉ dưỡng yên tĩnh, có thiết kế hiện đại, diện tích vừa phải, khung cảnh xanh mát và có không gian riêng tư là nơi nào. Hãy nêu tên homestay đó và giải thích lý do lựa chọn.</t>
+  </si>
+  <si>
+    <t>Homestay phù hợp nhất cho nhu cầu của một cặp đôi muốn nghỉ dưỡng yên tĩnh, thiết kế hiện đại, diện tích nhỏ gọn và có không gian riêng tư là Nhà Log Homestay Sóc Sơn.
+Lý do:
+Nhà Log Homestay nằm tại Lâm Trường, Sóc Sơn, sở hữu thiết kế hiện đại, là điểm nổi bật được nhiều bạn trẻ yêu thích.
+Mỗi căn nhà thuộc tổ hợp Nhà Log có diện tích nhỏ (khoảng 17m2), phù hợp cho 2 người lớn với giường đôi 1m6x2m.
+Không gian xanh mát, bao quanh bởi nhiều cây xanh, tạo cảm giác yên tĩnh, gần gũi với thiên nhiên.
+Mỗi căn đều có nhiều cửa kính lớn, tận dụng tối đa ánh sáng tự nhiên và nhìn thẳng ra khu vườn—tạo không gian riêng tư và thư giãn.
+Tất cả căn hộ đều có nhà vệ sinh khép kín, đảm bảo sự riêng tư.
+Mái hiên và bộ bàn ghế nhỏ giúp cặp đôi có thể thưởng thức bữa ăn, ngắm cảnh và tận hưởng sự bình yên.
+Dựa trên các tiêu chí “yên tĩnh – riêng tư – thiết kế hiện đại – diện tích nhỏ – bao quanh thiên nhiên”, Nhà Log Homestay Sóc Sơn đáp ứng đầy đủ nhất trong các homestay Sóc Sơn được liệt kê trong dữ liệu.</t>
+  </si>
+  <si>
+    <t>Khách sạn Hà Nội Daewoo nằm ở đâu?</t>
+  </si>
+  <si>
+    <t>Khách sạn Hà Nội Daewoo nằm tại địa chỉ: 360 Kim Mã, phường Ngọc Khánh, quận Ba Đình, thành phố Hà Nội.</t>
+  </si>
+  <si>
+    <t>Trong danh sách các nhà nghỉ giá rẻ ở Hà Nội, đâu là nhà nghỉ có mức giá khoảng 250.000–300.000 VNĐ/đêm và nằm tại khu vực Hà Đông?</t>
+  </si>
+  <si>
+    <t>Nhà nghỉ phù hợp với mức giá 250.000–300.000 VNĐ/đêm và nằm tại Hà Đông là:
+Xala Night Guest House
+Địa chỉ: Khu Xala, Hà Đông, Hà Nội
+Giá tham khảo: 250.000 VNĐ/đêm
+Mô tả dựa trên dữ liệu: Nhà nghỉ nằm tại khu phố sầm uất của Hà Đông, thiết kế chủ đạo màu trắng kết hợp hoa văn độc đáo, phòng ốc hiện đại, đầy đủ tiện nghi và mức giá rất hợp lý cho các chuyến lưu trú ngắn ngày.</t>
+  </si>
+  <si>
+    <t>Trong các nhà nghỉ gần sân bay Nội Bài, đâu là nơi có mức giá khoảng 240.000–300.000đ/đêm và nằm ở khu vực Sóc Sơn?</t>
+  </si>
+  <si>
+    <t>Trong danh sách nhà nghỉ/khách sạn gần sân bay Nội Bài, có hai địa điểm nằm tại Sóc Sơn và có mức giá trong khoảng 240.000–300.000đ/đêm:
+1) Ánh Dương Hotel
+Địa chỉ: 19 Đ. Võ Văn Kiệt, Điền Xá, Sóc Sơn, Hà Nội
+Giá phòng: Từ 240.000đ/đêm
+Theo dữ liệu: Khách sạn thiết kế đơn giản nhưng sang trọng, có phòng đơn và phòng đôi, đầy đủ tiện nghi như tivi, điều hòa, wifi miễn phí, khu hiên rộng rãi.
+2) Thanh Hương Airport Hotel
+Địa chỉ: Thôn Điền Xá, xã Quang Tiến, huyện Sóc Sơn
+Giá phòng: Từ 240.000đ/đêm
+Theo dữ liệu: Khách sạn cách sân bay Nội Bài 4,1 km, phòng rộng rãi, đầy đủ tiện nghi (máy lạnh, két an toàn, tivi, phòng tắm riêng), kèm dịch vụ bể bơi trong nhà và đưa đón sân bay.</t>
+  </si>
+  <si>
+    <t>Tôi muốn tìm một khách sạn cao cấp nằm gần Hồ Hoàn Kiếm, thì khách sạn nào phù hợp?</t>
+  </si>
+  <si>
+    <t>Các khách sạn cao cấp (từ 4–5 sao) nằm gần Hồ Hoàn Kiếm bao gồm:
+1) Sofitel Legend Metropole Hanoi (5 sao)
+Địa chỉ: 15 Ngô Quyền, quận Hoàn Kiếm
+Dữ liệu mô tả: Nằm ngay trung tâm thành phố, gần Nhà hát Lớn và nhiều điểm du lịch nổi tiếng khu vực hồ.
+2) The Oriental Jade Hotel &amp; Spa (5 sao)
+Địa chỉ: 92–94 Hàng Trống, quận Hoàn Kiếm
+Dữ liệu mô tả: Nằm tại phố cổ Hà Nội, có thể đi bộ đến Tràng Tiền Plaza, Nhà thờ Thánh Joseph và Nhà hát Lớn — đều thuộc khu vực quanh Hồ Hoàn Kiếm.
+3) Khách sạn Apricot Hà Nội (5 sao)
+Địa chỉ: 136 Hàng Trống, quận Hoàn Kiếm
+Dữ liệu mô tả: Nằm ở vị trí thuận tiện để di chuyển đến Nhà hát Múa rối Nước Thăng Long, Nhà thờ Lớn Hà Nội — đều nằm sát Hồ Hoàn Kiếm.
+4) Avani Central Hanoi Hotel (4 sao)
+Địa chỉ: 22A Quán Sứ, Hàng Bông, Hoàn Kiếm
+Dữ liệu mô tả: Gần Ga Hà Nội, Nhà tù Hỏa Lò, Cột cờ Hà Nội — thuộc khu vực trung tâm gần hồ.
+5) Serene Central Hotel (4 sao)
+Địa chỉ: 106 Hàng Bông, quận Hoàn Kiếm
+Dữ liệu mô tả: Nằm gần trung tâm phố cổ, chỉ vài phút đến các khu vực trung tâm Hoàn Kiếm.
+6) Hanoi Center Silk Classic Hotel &amp; Travel (4 sao)
+Địa chỉ: 41 Bát Sứ, Hoàn Kiếm
+Dữ liệu mô tả: Thuận tiện khám phá Tạ Hiện, chợ Đồng Xuân, Nhà hát Múa rối Thăng Long — nằm quanh Hồ Hoàn Kiếm.
+7) Hanoi Morning Hotel (3 sao – nhưng mô tả là nằm ngay khu vực trung tâm hồ)
+Địa chỉ: 10 Hàng Hành, Hoàn Kiếm
+Dữ liệu mô tả: Khách sạn phố cổ với tầm nhìn hướng ra hồ Hoàn Kiếm.</t>
+  </si>
+  <si>
+    <t>Tôi muốn tìm khách sạn nằm gần Hồ Hoàn Kiếm và có thể đi bộ đến Đền Ngọc Sơn. Thì những khách sạn nào phù hợp?</t>
+  </si>
+  <si>
+    <t>Các khách sạn có mô tả “gần Hồ Hoàn Kiếm” và “gần Đền Ngọc Sơn” gồm:
+1) Rex Hà Nội Hotel (4 sao)
+•	Địa chỉ: 42–44 Gia Ngư, Hàng Bạc, Hoàn Kiếm.
+•	Dữ liệu mô tả:
+Chỉ cách Hồ Hoàn Kiếm, Đền Ngọc Sơn, Ô Quan Chưởng vài phút đi bộ.
+Nằm giữa lòng Phố Cổ Hà Nội.
+2) Hà Nội Pearl Hotel (4 sao)
+•	Địa chỉ: 6 Báo Khánh, Hàng Trống, Hoàn Kiếm.
+•	Dữ liệu mô tả:
+“Chỉ cách Hồ Hoàn Kiếm vài bước chân.”
+Điểm gần gồm: Phố đi bộ, Đền Ngọc Sơn, Nhà Thờ Lớn, Nhà hát múa rối nước.
+3) Authentic Hà Nội Hotel (4 sao)
+•	Địa chỉ: 13 Lý Thái Tổ, Hoàn Kiếm.
+•	Dữ liệu mô tả:
+Chỉ cách Hồ Hoàn Kiếm, Nhà Thờ Lớn, Nhà Hát Lớn vài phút di chuyển.
+Điểm gần: Đền Ngọc Sơn, Phố Đi Bộ.
+4) Silk Path Luxury Hà Nội Hotel (4 sao)
+•	Địa chỉ: 199 Hàng Bông, Hoàn Kiếm.
+•	Dữ liệu mô tả:
+Đi bộ vài phút là đến Hồ Hoàn Kiếm, Đền Ngọc Sơn, Nhà Thờ Lớn, Phố Đi Bộ.
+5) Mường Thanh Grand Hà Nội Centre Hotel (4 sao)
+•	Địa chỉ: 78 Thợ Nhuộm, Hoàn Kiếm.
+•	Dữ liệu mô tả:
+“Chỉ cách Hồ Hoàn Kiếm và khu phố cổ vài phút đi bộ.”
+Điểm gần: Đền Ngọc Sơn, Hồ Gươm.</t>
+  </si>
+  <si>
+    <t>Zéphyr Hotel Hà Nội nằm ở đâu và hạng sao bao nhiêu?</t>
+  </si>
+  <si>
+    <t>Zéphyr Hotel Hà Nội nằm tại số 4 – 6 Bà Triệu, Phường Tràng Tiền, Quận Hoàn Kiếm, Hà Nội và là khách sạn 4 sao.</t>
+  </si>
+  <si>
+    <t>Top 10 khách sạn thương gia tại Hà Nội – đẳng cấp, chuyên nghiệp</t>
+  </si>
+  <si>
+    <t>Top 10 khách sạn thương gia tại Hà Nội gồm:
+Lotte Hotel Hà Nội
+Pan Pacific Hanoi Hotel
+Meliá Hà Nội Hotel
+Sofitel Legend Metropole Hà Nội
+Grand Vista Hotel Hà Nội
+Dolce by Wyndham Hà Nội Golden Lake
+InterContinental Hanoi Westlake
+Apricot Hotel Hà Nội
+Pullman Hà Nội Hotel</t>
+  </si>
+  <si>
+    <t>Những khách sạn 3 sao nào gần Hồ Tây có dịch vụ và tiện nghi tốt?</t>
+  </si>
+  <si>
+    <t>khách sạn 3 sao gần Hồ Tây có dịch vụ và tiện nghi tốt:
+1) Sunset Westlake Hà Nội
+Địa chỉ: 491-493 Lạc Long Quân, Phường Xuân La, Quận Tây Hồ, Hà Nội
+Hạng sao: 3 sao
+Điểm đánh giá: 9.7/10
+Tiện nghi &amp; dịch vụ nổi bật:
+Tầm nhìn đẹp ra Hồ Tây và thành phố
+Spa: mát-xa, xông hơi khô, bồn tắm nước nóng
+Nhà hàng Sunset &amp; Sunset Bar với thực đơn Việt – quốc tế, buffet tối phong phú
+Các điểm tham quan gần: Hồ Tây, Bảo tàng Dân tộc học Việt Nam, Chùa Trấn Quốc, Lăng Bác, Chùa Một Cột
+2) Lake View Apartment &amp; Hotel Hà Nội
+Địa chỉ: 65 Phố Trích Sài, Phường Bưởi, Quận Tây Hồ, Hà Nội
+Hạng sao: 3 sao
+Điểm đánh giá: 9.8/10
+Tiện nghi &amp; dịch vụ nổi bật:
+Vị trí ngay bên bờ Hồ Tây
+Thiết kế hiện đại, sang trọng
+Phòng rộng rãi, tầm nhìn hướng Hồ Tây
+Các điểm tham quan gần: Hồ Tây, Bảo tàng Dân tộc học Việt Nam, Chùa Một Cột, Lăng Bác, Chùa Trấn Quốc
+3) Oriental Palace Apartments Hà Nội
+Địa chỉ: 33 Tây Hồ, Phường Quảng An, Quận Tây Hồ, Hà Nội
+Hạng sao: 3 sao
+Điểm đánh giá: 9.3/10
+Tiện nghi &amp; dịch vụ nổi bật:
+Nhà hàng, hồ bơi ngoài trời theo mùa, phòng xông hơi
+Chỗ đỗ xe riêng miễn phí
+Bữa sáng tự chọn hoặc kiểu Mỹ
+Các điểm tham quan gần: Hồ Tây, Đền Quán Thánh, Chợ Đồng Xuân, Ô Quan Chưởng, Nhà hát múa rối nước Thăng Long</t>
+  </si>
+  <si>
+    <t>Top 10 khách sạn trung tâm Hà Nội là những khách sạn nào?</t>
+  </si>
+  <si>
+    <t>danh sách gồm 10 khách sạn sau:
+Sofitel Legend Metropole Hà Nội
+Địa chỉ: Số 15 Ngô Quyền, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 3.970.000 VNĐ/phòng/đêm
+Hotel Mercure Hà Nội la Gare
+Địa chỉ: Số 94 Lý Thường Kiệt, Cửa Nam, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 973.000 VNĐ/phòng/đêm
+Golden Rooster Hotel and Spa Hà Nội
+Địa chỉ: Số 17 Hàng Gà, Hàng Bồ, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 900.000 VNĐ/phòng/đêm
+Mövenpick Hà Nội
+Địa chỉ: Số 83A Lý Thường Kiệt, Cửa Nam, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 755.000 VNĐ/phòng/đêm
+Hà Nội Allure Hotel
+Địa chỉ: Số 52 Đào Duy Từ, Hàng Buồm, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 800.000 VNĐ/phòng/đêm
+Hotel Hà Nội Tirant
+Địa chỉ: Số 38 Phố Gia Ngư, Hàng Bạc, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 364.000 VNĐ/phòng/đêm
+Anatole Hotel Hà Nội
+Địa chỉ: Số 26–28–30 Nhà Chung, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 155.000 VNĐ/phòng/đêm
+Hà Nội La Sinfonía Del Rey Hotel &amp; Spa
+Địa chỉ: Số 33–35 Hàng Dầu, Lý Thái Tổ, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 949.000 VNĐ/phòng/đêm
+Apricot Hotel Hà Nội
+Địa chỉ: Số 136 Hàng Trống, Hoàn Kiếm, Hà Nội
+Giá tham khảo: 750.000 VNĐ/phòng/đêm</t>
+  </si>
+  <si>
+    <t>Những địa điểm nào phù hợp cho hoạt động cắm trại hoặc picnic cuối tuần?</t>
+  </si>
+  <si>
+    <t>các địa điểm phù hợp cho hoạt động cắm trại hoặc picnic cuối tuần gồm:
+1. Công Viên Yên Sở – Điểm Đến Xanh Mát Cho Cuối Tuần Thư Giãn
+Được ví như lá phổi xanh của thủ đô.
+Không gian rộng lớn, thoáng đãng, trong lành.
+Có hồ nước mênh mông, thảm cỏ trải dài và lối đi rợp bóng cây.
+Là địa điểm lý tưởng cho dạo bộ, đạp xe, picnic cùng gia đình, hoặc tận hưởng yên tĩnh để “nạp năng lượng”.
+Có nhiều góc check-in sống ảo như cầu gỗ, vườn hoa.
+2. Thung Lũng Bản Xôi – Thiên Đường Nghỉ Dưỡng Giữa Núi Rừng Ba Vì
+Cách Hà Nội hơn 40 km.
+Khung cảnh thiên nhiên hoang sơ, thơ mộng với núi rừng trùng điệp, thảm cỏ xanh và mặt hồ mênh mông.
+Bầu không khí trong lành, mát mẻ, thích hợp để tránh xa phố thị.
+Rất phù hợp cho các hoạt động cắm trại, picnic, teambuilding, nướng BBQ bên hồ.
+Buổi sớm hoặc hoàng hôn mang vẻ đẹp đặc biệt thơ mộng.
+3. Thung Lũng Xanh – Hồ Kèo Cà (Sóc Sơn) – “Đà Lạt” Của Hà Nội
+Cách Hà Nội khoảng 30 km.
+Không gian tự nhiên trong lành, mát mẻ.
+Là nơi để hòa mình vào thiên nhiên, tạm rời xa lo toan.
+Rất lý tưởng cho cắm trại cuối tuần.
+Du khách có thể trải nghiệm câu cá, chèo sup, ngắm mây trời và tận hưởng nhịp sống chậm.
+4. Đồi Bù (Hà Nội) – Thiên Đường Dù Lượn, Săn Mây
+Nằm trong nhóm địa điểm gần Hà Nội dành cho trải nghiệm ngoài trời.
+Là nơi nổi tiếng với dù lượn và săn mây.
+Hoạt động ngoài trời phù hợp cho một chuyến đi cuối tuần kết hợp thiên nhiên và vận động.</t>
+  </si>
+  <si>
+    <t>Tết Nguyên Đán diễn ra vào khoảng từ cuối tháng 1 đến giữa tháng 2 dương lịch (dựa trên âm lịch). Về chính thức, kỳ nghỉ Tết kéo dài ba ngày, nhưng các hoạt động lễ hội thường kéo dài tới một tuần hoặc hơn và không khí chuẩn bị đã bắt đầu từ sớm.</t>
+  </si>
+  <si>
+    <t>Tết Nguyên Đán (Tet Holiday) thường diễn ra vào thời gian nào trong năm và chính thức được nghỉ bao lâu?</t>
+  </si>
+  <si>
+    <t>Lễ hội Gióng (Giong Festival) được tổ chức vào ngày nào theo âm lịch và tại đâu ở Hà Nội?</t>
+  </si>
+  <si>
+    <t>Lễ hội Gióng được tổ chức từ ngày mồng 6 đến mồng 8 tháng Giêng âm lịch tại đền Sóc trên núi Vệ Linh, huyện Sóc Sơn, Hà Nội.</t>
+  </si>
+  <si>
+    <t>Hội Đống Đa kỷ niệm chiến thắng nào và gắn với vị hoàng đế nào của Việt Nam?</t>
+  </si>
+  <si>
+    <t>Hội Đống Đa kỷ niệm chiến thắng Ngọc Hồi – Đống Đa và gắn với Hoàng đế Quang Trung, người lãnh đạo cuộc kháng chiến chống ngoại xâm lừng lẫy này.</t>
+  </si>
+  <si>
+    <t>Hội làng nào ở Thanh Trì tôn vinh nghề dệt và ghi nhớ công lao của Phùng Hưng?</t>
+  </si>
+  <si>
+    <t>Đó là hội làng Triều Khúc, thuộc làng Triều Khúc, huyện Thanh Trì. Lễ hội nhằm ghi nhớ công ơn người anh hùng dân tộc Phùng Hưng và tôn vinh nghề dệt của làng.</t>
+  </si>
+  <si>
+    <t>Mô tả các nghi lễ và hoạt động chính của Giong Festival (lễ hội Gióng).</t>
+  </si>
+  <si>
+    <t>Giong Festival được tổ chức từ ngày 6–8 tháng Giêng âm lịch tại đền Sóc trên núi Vệ Linh, huyện Sóc Sơn. Đây là một trong những lễ hội lâu đời và được tôn kính nhất ở Hà Nội, được UNESCO công nhận là di sản văn hóa phi vật thể. Lễ hội tưởng niệm Thánh Gióng – vị anh hùng huyền thoại. Các hoạt động chính gồm những nghi lễ linh thiêng như rước kiệu, tắm tượng, làm sạch tượng, dâng hương và các nghi thức cúng tế. Bên cạnh đó còn có nhiều trò chơi dân gian, tiết mục biểu diễn truyền thống, giúp du khách trải nghiệm sâu sắc giá trị văn hóa và lịch sử của Việt Nam.</t>
+  </si>
+  <si>
+    <t>Trình bày hành trình và không khí lễ hội tại Perfume Pagoda Festival (lễ hội Chùa Hương).</t>
+  </si>
+  <si>
+    <t>Lễ hội Chùa Hương diễn ra từ ngày mồng 6 tháng Giêng tới tận tháng Ba âm lịch tại quần thể Chùa Hương, huyện Mỹ Đức. Hành trình đến Chùa Hương là một chuyến du lịch tâm linh giữa khung cảnh thiên nhiên hùng vĩ: du khách đi qua núi non, cánh đồng lúa và các hang động đá vôi để đến được ngôi chùa. Trong thời gian lễ hội, không gian được trang hoàng rực rỡ với những đồ trang trí nhiều màu sắc và ánh nến lung linh, cùng các nghi lễ tâm linh được tổ chức thường xuyên. Lễ hội mang đến sự kết hợp giữa vẻ đẹp thiên nhiên và những truyền thống văn hóa, tôn giáo lâu đời, tạo nên một trải nghiệm đặc biệt cho người tham dự.</t>
+  </si>
+  <si>
+    <t>So sánh điểm nhấn văn hóa và hoạt động tiêu biểu của Bat Trang Pottery Village Festival và Vong La Festival.</t>
+  </si>
+  <si>
+    <t>Bat Trang Pottery Village Festival diễn ra từ ngày 14–16 tháng Hai âm lịch tại làng gốm Bát Tràng, huyện Gia Lâm. Lễ hội tôn vinh truyền thống làm gốm lâu đời của làng. Du khách có thể xem các nghệ nhân trình diễn kỹ thuật làm gốm, tham gia các tiết mục văn hóa và cùng cộng đồng cầu nguyện cho hòa bình, thịnh vượng. Điểm nhấn là nghề gốm và tay nghề của thợ gốm Bát Tràng. Vong La Festival diễn ra từ ngày 13–15 tháng Giêng âm lịch tại đền Đại Độ, huyện Đông Anh. Đây là lễ hội rực rỡ với cờ phướn, trang trí nhiều màu sắc, nổi bật với các tiết mục hát Quan họ và múa lân sôi động. Trọng tâm của lễ hội Vong La là không khí hội hè vui tươi, âm nhạc dân gian và các màn trình diễn tạo nên khung cảnh lễ hội sinh động. Như vậy, Bát Tràng nhấn mạnh nghề gốm truyền thống, còn Vòng La nổi bật bởi không khí lễ hội rực rỡ và các tiết mục Quan họ, múa lân.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trình bày ý nghĩa lịch sử và các hoạt động văn hóa chính của Co Loa Citadel Festival/Hội Cổ Loa </t>
+  </si>
+  <si>
+    <t>Hội Cổ Loa diễn ra từ ngày 6 đến ngày 16 tháng Giêng âm lịch để tưởng nhớ Thục Phán An Dương Vương, người được vua Hùng thứ 18 nhường ngôi và là vị vua lập nên nước Âu Lạc cổ. Lễ hội gắn với truyền thuyết Nỏ Thần và chuyện tình Mỵ Châu – Trọng Thủy. Trong phần lễ có đám rước thần của 12 xóm. Phần hội tổ chức nhiều trò chơi dân gian như thi thổi cơm, chơi đu, hát chèo… Theo mô tả tiếng Anh, Co Loa Citadel Festival được tổ chức tại chùa An Dương Vương ở huyện Đông Anh, với các tiết mục hát Quan họ, múa rối nước và nhiều hoạt động văn hóa khác. Tất cả nhằm tôn vinh di sản của vua An Dương Vương và ý nghĩa lịch sử của thành Cổ Loa.</t>
+  </si>
+  <si>
+    <t>Mô tả đầy đủ ý nghĩa và không khí của lễ hội Trung Thu (Mid-Autumn Festival) tại Hà Nội.</t>
+  </si>
+  <si>
+    <t>Trung Thu diễn ra vào ngày 15 tháng 8 âm lịch và là dịp đoàn tụ gia đình, đặc biệt ý nghĩa với trẻ em. Lễ hội gắn với mùa thu hoạch, sự gắn kết gia đình và các truyền thuyết về chị Hằng (Moon Lady – Hằng Nga) và chú Cuội (Moon Boy – Cuội). Vài tuần trước Trung Thu, Hà Nội trở thành một \"thế giới lễ hội\": đường phố và các khu chợ tràn ngập đèn lồng rực rỡ, bánh trung thu và đồ chơi. Các gia đình chuẩn bị cho đêm hội bằng cách làm hoặc mua các món ăn truyền thống và trang trí nhà cửa bằng đèn lồng và các họa tiết về trăng. Đêm Trung Thu là một lễ hội vui tươi, nơi mọi người quây quần dưới ánh trăng rằm, thưởng thức bánh, ngắm đèn lồng và tham gia các hoạt động văn hóa, thể hiện sự ấm áp, đoàn kết trong truyền thống Việt Nam.</t>
+  </si>
+  <si>
+    <t>Hội đền Hai Bà Trưng được mở từ ngày nào đến ngày nào theo âm lịch để tưởng nhớ công ơn Hai Bà?</t>
+  </si>
+  <si>
+    <t>Hội đền Hai Bà Trưng được mở hằng năm từ mồng 3 tới mồng 6 tháng Hai âm lịch để tưởng nhớ công ơn Hai Bà Trưng.</t>
+  </si>
+  <si>
+    <t>Di chuyển bằng xe buýt từ sân bay Nội Bài vào trung tâm Hà Nội có giá khoảng bao nhiêu?</t>
+  </si>
+  <si>
+    <t>Giá xe buýt từ sân bay Nội Bài vào trung tâm Hà Nội khoảng 35.000 – 40.000 VNĐ/lượt, với các tuyến phổ biến là tuyến 86 (Nội Bài – ga Hà Nội) và tuyến 17 (Nội Bài – Long Biên).</t>
+  </si>
+  <si>
+    <t>Giá thuê xe máy trong nội thành Hà Nội một ngày là bao nhiêu?</t>
+  </si>
+  <si>
+    <t>Giá thuê xe máy trong nội thành Hà Nội khoảng 100.000 – 200.000 VNĐ/ngày, tùy loại xe.</t>
+  </si>
+  <si>
+    <t>Tuyến Metro duy nhất đang hoạt động ở Hà Nội là tuyến nào?</t>
+  </si>
+  <si>
+    <t>Tuyến Metro duy nhất đang hoạt động là tuyến 2A: Cát Linh – Yên Nghĩa, dài khoảng 12 km.</t>
+  </si>
+  <si>
+    <t>Giá vé xe buýt nội thành Hà Nội dao động trong khoảng nào?</t>
+  </si>
+  <si>
+    <t>Xe buýt nội thành Hà Nội có giá 7.000 – 10.000 VNĐ/lượt.</t>
+  </si>
+  <si>
+    <t>Giá xe đưa đón sân bay (4 chỗ) từ Nội Bài về trung tâm Hà Nội khoảng bao nhiêu?</t>
+  </si>
+  <si>
+    <t>Xe đưa đón sân bay 4 chỗ có giá 250.000 – 350.000 VNĐ/xe, tùy hãng và thời điểm.</t>
+  </si>
+  <si>
+    <t>Các phương tiện di chuyển từ sân bay Nội Bài vào trung tâm thành phố.</t>
+  </si>
+  <si>
+    <t>Có ba phương tiện chính:
+Xe đưa đón sân bay: tiện lợi nhất, đặc biệt khi mang nhiều hành lý. Giá 250.000 – 350.000 VNĐ/xe. Nên đặt trước để tránh hết xe hoặc bị ép giá.
+Xe buýt: lựa chọn tiết kiệm nhất, với tuyến 86 (Nội Bài – ga Hà Nội) và 17 (Nội Bài – Long Biên). Giá 35.000 – 40.000 VNĐ/lượt.
+Taxi: nhanh nhưng chi phí cao hơn. Giá 300.000 – 400.000 VNĐ/xe, nên chọn hãng uy tín như Mai Linh, G7, Taxi Group.</t>
+  </si>
+  <si>
+    <t>Các lựa chọn di chuyển trong nội thành Hà Nội</t>
+  </si>
+  <si>
+    <t>Các lựa chọn gồm:
+Xe buýt: mạng lưới rộng, giá 7.000 – 10.000 VNĐ/lượt, nên dùng app hoặc bản đồ xe buýt.
+Taxi / xe công nghệ (Grab, Be): tiện lợi khi đi nhóm hoặc mang đồ; giá tính theo km.
+Xe máy thuê: linh hoạt khám phá Hà Nội, giá 100.000 – 200.000 VNĐ/ngày.
+Xích lô: phù hợp ngắm phố cổ, giá 100.000 – 200.000 VNĐ/giờ.
+Thuê xe riêng: tùy loại xe và thời gian thuê; nên đặt trước.
+Grab / Gojek / Be: tiết kiệm và nhanh, Grab phổ biến nhất nhưng giá hơi cao hơn.
+Metro 2A: giá vé theo lượt 8.000 – 15.000 VNĐ, hoặc vé ngày 30.000 VNĐ.
+Xe đạp: giá 50.000 – 100.000 VNĐ/ngày, phù hợp khu phố cổ.
+Đi bộ: phù hợp dạo quanh 36 phố phường.
+Xe buýt hai tầng (mui trần): giá 130.000 – 599.000 VNĐ, đưa đến nhiều điểm du lịch nổi tiếng.</t>
+  </si>
+  <si>
+    <t>Chi tiết ưu – nhược điểm và mức giá các ứng dụng gọi xe (Grab, Gojek, Be) tại Hà Nội theo dữ liệu.</t>
+  </si>
+  <si>
+    <t>Có ba ứng dụng: Grab, Gojek, Be.
+Đây là dịch vụ hoạt động mạnh, được người dùng tin cậy vì tiết kiệm thời gian và chi phí so với taxi truyền thống.
+Grab được dùng nhiều nhất nên thời gian chờ ngắn, nhưng giá thường cao hơn hai ứng dụng còn lại.
+Lời khuyên: nên cài cả ba ứng dụng để so sánh giá trước khi đặt.
+Lưu ý ngoại lệ: khi di chuyển giữa Nội Bài và trung tâm thành phố, taxi truyền thống rẻ hơn và luôn có sẵn tại sân bay.</t>
+  </si>
+  <si>
+    <t>Mô tả toàn bộ thông tin liên quan đến việc thuê xe máy khi đi Hà Nội</t>
+  </si>
+  <si>
+    <t>Giá thuê 100.000 – 200.000 VNĐ/ngày (tùy loại xe).
+Có thể thuê trực tiếp tại nơi lưu trú hoặc cửa hàng gần đó; có dịch vụ giao xe tận nơi.
+Cần bằng lái xe và tốt nhất là có bảo hiểm du lịch.
+Thông thường không cần đặt cọc, nhưng đôi khi có thể yêu cầu đặt cọc nhỏ, trả trước, hoặc chụp ảnh hộ chiếu.
+Lời khuyên khi phượt xe máy từ tỉnh lân cận:
+chuẩn bị thể lực, kiểm tra xe (phanh, xăng, máy),
+đi theo nhóm,
+đội nón bảo hiểm, dùng chống nắng, mang theo nước và đồ ăn nhanh.</t>
+  </si>
+  <si>
+    <t>các tuyến xe buýt hoặc điểm đến quan trọng khi sử dụng xe buýt trong nội thành hoặc từ các điểm du lịch ở Hà Nội</t>
+  </si>
+  <si>
+    <t>Trong dữ liệu có các tuyến/điểm nổi bật:
+Tuyến đi Hồ Gươm: 9, 14, 36.
+Tuyến đi chợ Đồng Xuân: 31.
+Tuyến đi Ô Quan Chưởng: 03, 11, 14, 22, 18, 34, 40.
+Xe buýt sân bay: 86, 17.
+Xe buýt mui trần: đưa đến phố cổ, Nhà thờ lớn, Cột cờ – bảo tàng lịch sử quân sự, Lăng Chủ tịch, Chùa Một Cột, Quốc Hội, Hồ Tây, Trấn Quốc, Cửa Bắc, Hoàng Thành Thăng Long, Văn Miếu, Hỏa Lò, Nhà hát lớn và nhiều điểm khác.</t>
   </si>
 </sst>
 </file>
@@ -563,8 +966,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -765,46 +1168,305 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="26" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="27" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="28" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="29" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="30" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="31" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="32" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="33" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="34" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="35" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="36" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="37" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="38" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="39" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="40" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="41" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="42" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="43" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="44" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="45" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="46" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="47" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="48" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="49" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="50" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="51" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="52" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="56" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="57" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="61" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="62" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="65" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="66" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="67" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
separate API for reranker with pinecone
</commit_message>
<xml_diff>
--- a/evaluate/data/data_evaluate_Hanoi.xlsx
+++ b/evaluate/data/data_evaluate_Hanoi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDTU\Year_4_Semester1\Dự án\Code\evaluate\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D3CBDD-83B6-464F-817A-4BC1B095C052}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AA467-B91F-403D-A66B-C53F5A640B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>Question</t>
   </si>
@@ -595,6 +595,56 @@
 Tuyến đi Ô Quan Chưởng: 03, 11, 14, 22, 18, 34, 40.
 Xe buýt sân bay: 86, 17.
 Xe buýt mui trần: đưa đến phố cổ, Nhà thờ lớn, Cột cờ – bảo tàng lịch sử quân sự, Lăng Chủ tịch, Chùa Một Cột, Quốc Hội, Hồ Tây, Trấn Quốc, Cửa Bắc, Hoàng Thành Thăng Long, Văn Miếu, Hỏa Lò, Nhà hát lớn và nhiều điểm khác.</t>
+  </si>
+  <si>
+    <t>Nhà hàng Nét Huế Hà Nội chuyên phục vụ đặc sản của vùng miền nào?</t>
+  </si>
+  <si>
+    <t>Nhà hàng Nét Huế Hà Nội chuyên phục vụ các món đặc sản Huế, mang đậm hương vị ẩm thực miền Trung như bún bò Huế, bánh khoái, bánh nậm,…</t>
+  </si>
+  <si>
+    <t>Nhà Hàng Hibana By Koki ở Hà Nội có địa chỉ ở đâu?</t>
+  </si>
+  <si>
+    <t>Nhà Hàng Hibana By Koki có địa chỉ tại số 11, đường Lê Phụng Hiểu, quận Hoàn Kiếm, Hà Nội.</t>
+  </si>
+  <si>
+    <t>Nhà hàng Buffet Chef Dzung ở Hà Nội nằm ở đâu?</t>
+  </si>
+  <si>
+    <t>Nhà hàng Buffet Chef Dzung Hà Nội có địa chỉ tại 71 Đ. Nguyễn Chí Thanh, Thành Công, Đống Đa, Hà Nội.</t>
+  </si>
+  <si>
+    <t>Dimsum Corner Hà Nội nổi tiếng với điều gì và thực đơn của nhà hàng có những loại món nào?</t>
+  </si>
+  <si>
+    <t>Dimsum Corner Hà Nội nổi tiếng là một trong những nhà hàng dimsum được nhiều tín đồ ẩm thực Trung Hoa yêu thích. Nhà hàng chinh phục thực khách nhờ thực đơn đa dạng và chất lượng món ăn ổn định. Điểm nổi bật nhất là thực đơn phong phú với hơn 30 món dimsum truyền thống như các loại há cảo, xíu mại, bánh bao và các món chiên hấp dẫn. Ngoài dimsum, nhà hàng còn phục vụ các món Trung Hoa khác như cháo, mì, cơm và các món tráng miệng, giúp bữa ăn trở nên trọn vẹn.</t>
+  </si>
+  <si>
+    <t>ManWah Taiwanese Hotpot có gì nổi bật khiến thực khách Hà Nội yêu thích và nhà hàng phục vụ những loại nước lẩu cũng như topping nào?</t>
+  </si>
+  <si>
+    <t>ManWah Taiwanese Hotpot nổi bật bởi hương vị lẩu chuẩn Đài Loan, từ cay nồng đến thanh ngọt, đều rất đậm đà và cuốn hút. Tuy mới xuất hiện tại Việt Nam gần đây nhưng ManWah đã nhanh chóng thu hút thực khách nhờ hương vị đặc trưng này. Nhà hàng có đến 6 loại nước lẩu độc đáo phù hợp với nhiều sở thích khác nhau. Thực đơn của ManWah cũng rất đa dạng, với hơn 80 món topping, bao gồm các loại thịt bò, hải sản tươi ngon, cùng nhiều loại rau củ phong phú. Những yếu tố này mang đến một bữa lẩu đầy đủ và trọn vị, khiến ManWah trở thành lựa chọn yêu thích của nhiều tín đồ ẩm thực, đặc biệt trong những ngày gió mùa.</t>
+  </si>
+  <si>
+    <t>Lẩu Thái Deli Hà Nội có những cơ sở nào, giờ mở cửa ra sao và trải nghiệm ẩm thực mà quán mang lại được mô tả như thế nào?</t>
+  </si>
+  <si>
+    <t>Lẩu Thái Deli Hà Nội có các cơ sở tại:
+Ngõ 4 Hàm Nghi, Số 2 lô TT01, Moncity, Mỹ Đình
+B10, Biệt thự PANDORA, 53 Triều Khúc
+25 Vũ Ngọc Phan
+LK05 Biệt thự LACASA, Láng Hạ
+Số 5 Quan Hoa, Cầu Giấy
+Giờ mở cửa của Thái Deli là 11:00–14:00 và 17:00–23:00. Giá tham khảo ở đây nằm trong khoảng 100.000VNĐ – 160.000VNĐ/người.
+Trải nghiệm ẩm thực tại Thái Deli được mô tả là khiến thực khách vừa được chìm đắm trong không gian ấm cúng đậm nét văn hóa Thái, vừa thưởng thức hương vị ẩm thực chuẩn vị trứ danh Thái Lan. Khách đến đây sẽ có cảm giác thư giãn, thoải mái như đang lạc vào xứ sở Chùa Vàng, tách biệt khỏi náo nhiệt, đồng thời tận hưởng sự bùng nổ vị giác từ các món lẩu đặc trưng.</t>
+  </si>
+  <si>
+    <t>Lẩu cua đồng Song Hà ở Hà Nội có địa chỉ ở đâu, giờ mở cửa như thế nào, và món lẩu cua đồng tại đây được mô tả ra sao?</t>
+  </si>
+  <si>
+    <t>Lẩu cua đồng Song Hà ở Hà Nội có địa chỉ tại 685 Lạc Long Quân, Quận Tây Hồ, Hà Nội. Giờ mở cửa của quán là 8:00 - 22:00, với mức giá tham khảo từ 50.000VNĐ - 300.000VNĐ.
+Nước dùng lẩu cua đồng Song Hà được đảm bảo chế biến từ cua đồng 100%, vì vậy có vị ngọt thanh và mùi hương ngào ngạt đặc trưng của cua đồng. Khi nồi lẩu được mang ra, thực khách sẽ bị thu hút bởi nồi nước dùng nổi đầy gạch cua vàng óng, điểm thêm cà chua đỏ, đậu chiên vàng, cùng một chút hành lá và rau xanh. Để món lẩu cua đồng thêm trọn vẹn, quán phục vụ kèm bắp bò tươi, sườn sụn, nấm và các loại rau xanh khác, đầy đủ và hấp dẫn.</t>
   </si>
 </sst>
 </file>
@@ -966,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1464,25 +1514,74 @@
         <v>121</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="64" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="65" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="81" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="83" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Done evaluate for data Hanoi
</commit_message>
<xml_diff>
--- a/evaluate/data/data_evaluate_Hanoi.xlsx
+++ b/evaluate/data/data_evaluate_Hanoi.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TDTU\Year_4_Semester1\Dự án\Code\evaluate\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{140AA467-B91F-403D-A66B-C53F5A640B2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B741CAC-93CB-422A-BA39-652FAD8EB6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="202">
   <si>
     <t>Question</t>
   </si>
@@ -646,6 +655,254 @@
     <t>Lẩu cua đồng Song Hà ở Hà Nội có địa chỉ tại 685 Lạc Long Quân, Quận Tây Hồ, Hà Nội. Giờ mở cửa của quán là 8:00 - 22:00, với mức giá tham khảo từ 50.000VNĐ - 300.000VNĐ.
 Nước dùng lẩu cua đồng Song Hà được đảm bảo chế biến từ cua đồng 100%, vì vậy có vị ngọt thanh và mùi hương ngào ngạt đặc trưng của cua đồng. Khi nồi lẩu được mang ra, thực khách sẽ bị thu hút bởi nồi nước dùng nổi đầy gạch cua vàng óng, điểm thêm cà chua đỏ, đậu chiên vàng, cùng một chút hành lá và rau xanh. Để món lẩu cua đồng thêm trọn vẹn, quán phục vụ kèm bắp bò tươi, sườn sụn, nấm và các loại rau xanh khác, đầy đủ và hấp dẫn.</t>
   </si>
+  <si>
+    <t>Nhà hàng Michelin Hà Nội – Gia có địa chỉ ở đâu, mức giá và giờ mở cửa như thế nào, và điều gì làm cho trải nghiệm ẩm thực tại nhà hàng này trở nên đặc biệt?</t>
+  </si>
+  <si>
+    <t>Nhà hàng Michelin Hà Nội – Gia có địa chỉ tại 61 P. Văn Miếu, Văn Miếu, Đống Đa, Hà Nội. Mức giá tham khảo tại đây dao động khoảng 700.000 – 2.000.000 VNĐ cho set Tasting Menu.
+Giờ mở cửa của nhà hàng:
+Từ 18:00 – 21:00 (Thứ Ba – Thứ Năm)
+Từ 11:00 – 13:30 và 18:00 – 21:00 (Thứ Năm – Chủ Nhật)
+Điểm đặc biệt của Gia là phong cách phục vụ theo Tasting Menu 10 món ăn và đồ uống được sắp xếp trước, khách không chọn món theo menu truyền thống. Thực đơn được thay đổi theo mùa, mỗi 3 tháng một lần, nên khách hàng rất hiếm khi được ăn lại món cũ. Món ăn được trình bày tinh tế, tạo cảm giác mới mẻ và thú vị khi thưởng thức. Không gian nhà hàng nằm trong một ngôi nhà cổ gần 100 năm tuổi, mang đến cảm giác đẹp mắt, thân thiện và gần gũi như ở nhà.</t>
+  </si>
+  <si>
+    <t>Nhà hàng Bếp Prime ở Hà Nội có địa chỉ, mức giá và giờ mở cửa như thế nào? Ngoài ra, nhà hàng được mô tả có những điểm đặc sắc gì về không gian và món ăn?</t>
+  </si>
+  <si>
+    <t>Nhà hàng Bếp Prime có địa chỉ tại Số 12 Hàng Điếu, Quận Hoàn Kiếm, Hà Nội. Mức giá tại đây dao động từ 350.000 - 450.000 VNĐ/người. Giờ mở cửa của nhà hàng là 10h30 - 14h00 và 17h00 - 22h30.
+Bếp Prime là một trong số ít nhà hàng ở Hà Nội được Michelin đánh giá cao. Nhà hàng là sự kết hợp hài hòa giữa các yếu tố ẩm thực, cá tính đầu bếp và phong cách phục vụ chuyên nghiệp. Các món ăn được chế biến cân bằng hương vị, mang lại trải nghiệm ẩm thực khó quên. Không gian của nhà hàng ấm cúng và đậm chất Việt Nam, được trang trí với hình ảnh gánh hàng rong, tường vàng và đèn lồng truyền thống. Một món ăn đặc sắc nổi bật tại Bếp Prime là lẩu gà khiêu vũ bốc lửa, với hương vị thơm lừng mùi thảo mộc và nước lẩu ngọt thanh.</t>
+  </si>
+  <si>
+    <t>Duong’s Restaurant được Michelin Guide mô tả như thế nào, nhà hàng phục vụ các món gì trong menu, và thực khách có thêm lựa chọn trải nghiệm đặc biệt nào khi đến đây?</t>
+  </si>
+  <si>
+    <t>Duong’s Restaurant được Michelin Guide liệt kê như một sự tôn vinh ẩm thực Việt Nam, mang đến phong cách trình bày món ăn nâng tầm và tinh tế. Nhà hàng được điều hành bởi Chef Hoàng Dương, người đã tham gia Iron Chef Vietnam và Top Chef Vietnam, và nhà hàng được đặt theo tên của ông.
+Menu à la carte của Duong’s Restaurant bao gồm các món ăn đặc trưng của Hà Nội như: phở, bún chả, salad lá chuối, nem (spring rolls) và cá hấp gói lá chuối. Bên cạnh món Việt, nhà hàng cũng phục vụ một số món quốc tế như ức vịt (ăn kèm cam, truffle và cơm risotto thảo mộc). Ngoài ra, thực khách cũng có thể chọn set menu 4 món.
+Một lựa chọn trải nghiệm đặc biệt tại Duong’s Restaurant là tham gia các lớp học nấu ăn chuyên nghiệp của nhà hàng nếu thực khách muốn quay lại vào một dịp khác.</t>
+  </si>
+  <si>
+    <t>Lụa Vạn Phúc có đặc điểm gì nổi bật theo mô tả?</t>
+  </si>
+  <si>
+    <t>Lụa Vạn Phúc nổi tiếng từ xưa với nghề dệt lụa. Lụa ở đây mỏng, mềm, thoáng mát và rất nhẹ, khi mặc rất thoải mái, khác hẳn với các loại lụa thông thường.</t>
+  </si>
+  <si>
+    <t>Những thời điểm nào được xem là lý tưởng nhất để du lịch Hà Nội?</t>
+  </si>
+  <si>
+    <t>Thời điểm lý tưởng nhất để du lịch Hà Nội là mùa xuân từ tháng 2 đến tháng 4 và mùa thu từ tháng 9 đến tháng 10. Trong những giai đoạn này, thời tiết thường mát mẻ, dễ chịu, ít mưa, rất thuận lợi cho việc tham quan và trải nghiệm các hoạt động ngoài trời.</t>
+  </si>
+  <si>
+    <t>thời điểm nào được xem là tốt nhất để du lịch Hà Nội?</t>
+  </si>
+  <si>
+    <t>Thời điểm tốt nhất để du lịch Hà Nội là mùa thu (khoảng tháng 9 đến tháng 11) và mùa xuân (tháng 3 và tháng 4), khi thời tiết dễ chịu và nhiệt độ ôn hòa.</t>
+  </si>
+  <si>
+    <t>Thời điểm nào trong năm được xem là lý tưởng nhất để khám phá Hà Nội?</t>
+  </si>
+  <si>
+    <t>Thời điểm lý tưởng nhất để khám phá Hà Nội là mùa xuân (tháng 2 đến tháng 3) hoặc mùa thu (tháng 8 đến tháng 10) vì đây là các mùa có thời tiết dễ chịu, mát mẻ và ổn định hơn so với mùa hè nóng bức và mùa đông lạnh.</t>
+  </si>
+  <si>
+    <t>Thời điểm nào trong năm là đẹp nhất để tham quan Thủ đô Hà Nội?</t>
+  </si>
+  <si>
+    <t>Hà Nội có bốn mùa và mỗi mùa đều có nét đẹp riêng, vì vậy bạn có thể tham quan Hà Nội vào bất kỳ thời điểm nào trong năm.
+Mùa xuân (tháng 2 – tháng 4): thời tiết lạnh, có mưa phùn nhẹ; hoa xuân nở rộ.
+Mùa hè (tháng 5 – tháng 7): nắng nóng; người dân thường ra Hồ Tây hoặc vào công viên, trung tâm thương mại để giải nhiệt.
+Mùa thu (tháng 8 – tháng 10): lãng mạn, thơ mộng nhất; tràn ngập hoa sữa và hương lúa mới.
+Mùa đông (tháng 11 – tháng 1): rất lạnh nhưng mang vẻ đẹp trữ tình riêng.
+Vì vậy, mỗi mùa đều có vẻ đẹp riêng và có thể tham quan Hà Nội vào bất kỳ thời điểm nào trong năm.</t>
+  </si>
+  <si>
+    <t>Những đặc sản nào được gợi ý để mua làm quà khi du lịch Hà Nội?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">những đặc sản được gợi ý để mua làm quà khi du lịch Hà Nội gồm:
+Ô mai (Salted or Sugared Dried Fruits)
+Cốm (Green Rice Flakes)
+Trà sen (Lotus Tea)
+Lụa Vạn Phúc (Van Phuc Silk)
+Gốm Bát Tràng (Bat Trang Ceramics)
+</t>
+  </si>
+  <si>
+    <t>Khi du lịch Hà Nội, những món quà nào được gợi ý nên mua về?</t>
+  </si>
+  <si>
+    <t>những món quà được gợi ý nên mua khi du lịch Hà Nội gồm:
+Ô mai
+Cốm
+Trà sen
+Lụa Vạn Phúc
+Đồ gốm Bát Tràng</t>
+  </si>
+  <si>
+    <t>Khi đi du lịch Hà Nội, những món quà nào được gợi ý mua về?</t>
+  </si>
+  <si>
+    <t>ba món quà được gợi ý mua khi du lịch Hà Nội gồm:
+Bánh cốm Hàng Than – có hương cốm thơm cùng nhân đậu xanh bùi bùi, là món quà quê đặc biệt.
+Ô mai – đặc biệt là ô mai sấu, vị chua ngọt, được nhiều người chọn làm quà.
+Lụa Vạn Phúc – lụa mềm mại, thoáng mát, màu sắc tươi sáng, hoa văn đẹp; có thể mua tại làng Vạn Phúc hoặc các gian hàng trên phố Hàng Gai và Đinh Liệt.</t>
+  </si>
+  <si>
+    <t>những món quà nào được gợi ý nên mua khi du lịch Hà Nội?</t>
+  </si>
+  <si>
+    <t>các món quà nên mua khi du lịch Hà Nội gồm:
+Bánh cốm
+Trà sen
+Mận Hà Nội
+Chả cá Lã Vọng
+Ô mai
+Bánh chè lam
+Sấu
+Bánh chả
+Bưởi diễn
+Đồ gốm sứ
+Đồ thủ công mỹ nghệ
+Lụa
+Bánh khúc
+Chả rươi</t>
+  </si>
+  <si>
+    <t>10 Công ty du lịch uy tín chất lượng ở Hà Nội</t>
+  </si>
+  <si>
+    <t>10 Công ty du lịch uy tín chất lượng ở Hà Nội gồm:
+Công ty Smile Travel
+Công ty du lịch Vietravel
+Công ty du lịch VietFlame Tour
+Công ty Hoàng Việt Travel
+Công ty Bạch Dương Travel
+Công ty du lịch Best Price
+Công ty du lịch Quốc tế Đại Việt
+Công ty du lịch Khát Vọng Việt
+Công ty Elite Tour
+Công ty Bốn Mùa Tourist</t>
+  </si>
+  <si>
+    <t>Phở Hà Nội gồm những đặc điểm gì?</t>
+  </si>
+  <si>
+    <t>Phở Hà Nội có nước dùng trong, ngọt thanh, bánh phở mềm dai và thịt bò tươi ngon. Phở Hà Nội có nhiều loại như phở bò tái, phở bò chín, phở gà và phở chay.</t>
+  </si>
+  <si>
+    <t>Kem Tràng Tiền có những vị nào?</t>
+  </si>
+  <si>
+    <t>Kem Tràng Tiền có nhiều vị như vani, sô cô la và dâu tây. Kem có vị ngọt thanh, mát lạnh và thơm ngon.</t>
+  </si>
+  <si>
+    <t>Địa chỉ của Quán Phở 10 Lý Quốc Sư là gì?</t>
+  </si>
+  <si>
+    <t>Quán Phở 10 Lý Quốc Sư có địa chỉ: 10 Lý Quốc Sư, Phường Hàng Trống, Quận Hoàn Kiếm, Hà Nội, Việt Nam.</t>
+  </si>
+  <si>
+    <t>Cốm làng Vòng được làm từ loại lúa gì?</t>
+  </si>
+  <si>
+    <t>Cốm làng Vòng được làm từ lúa nếp cái hoa vàng, có màu xanh non, dẻo thơm và vị ngọt thanh.</t>
+  </si>
+  <si>
+    <t>Quán Bún Chả Hương Liên nổi tiếng với món gì?</t>
+  </si>
+  <si>
+    <t>Quán Bún Chả Hương Liên nổi tiếng với món Bún Chả “Obama” – từng được cựu Tổng thống Mỹ Barack Obama thưởng thức. Hương vị bún chả ở đây hài hòa, đậm đà với thịt nướng thơm lừng, chả viên mềm và nước chấm chua ngọt.</t>
+  </si>
+  <si>
+    <t>Hãy mô tả đầy đủ các thành phần và hương vị của món Bún Thang Hà Nội</t>
+  </si>
+  <si>
+    <t>Bún thang gồm bún, giò lụa, thịt gà, trứng gà, tôm khô và các nguyên liệu khác. Nước dùng của bún thang được ninh từ xương gà và tôm khô, có vị ngọt thanh và thơm ngon. Đây là món ăn cầu kỳ, tinh tế và đòi hỏi nhiều công phu chế biến.</t>
+  </si>
+  <si>
+    <t>Miêu tả hương vị và quy trình chế biến của Chả Cá Thăng Long</t>
+  </si>
+  <si>
+    <t>Chả Cá Thăng Long là món ăn đặc trưng của Hà Nội. Chả cá được ướp vàng ươm, nướng trên than hoa thơm lừng, ăn kèm bún, rau sống và mắm tôm. Miếng cá khi chín vàng hơi săn chắc, cháy cạnh giòn bên ngoài nhưng mềm ở giữa. Gia vị tẩm ướp vừa miệng và thơm phức. Khi ăn hòa quyện với mắm tôm tạo nên hương vị khó quên.</t>
+  </si>
+  <si>
+    <t>Hãy mô tả đặc điểm bánh cuốn tại Quán Bánh Cuốn Bà Xuân</t>
+  </si>
+  <si>
+    <t>Bánh cuốn Bà Xuân có lớp bánh mỏng tang, trắng mịn, được tráng ngay tại chỗ và luôn nóng hổi. Nhân gồm thịt băm và mộc nhĩ thơm ngậy. Hành phi vàng giòn được rắc lên trên. Nước chấm pha chua ngọt hài hòa, ăn kèm vài lát chả quế và chút tinh dầu cà cuống, tạo nên hương vị tròn trịa, tinh tế.</t>
+  </si>
+  <si>
+    <t>Nêu đầy đủ mô tả về hương vị và trải nghiệm tại Quán Xôi Mây Vọng Đức</t>
+  </si>
+  <si>
+    <t>Xôi Mây nổi tiếng gần 30 năm ở Hà Nội, có hương vị thơm ngon đặc trưng. Món xôi xéo có sắc vàng tươi, đậu xanh chín mềm, hành phi vàng sậm giòn béo nằm trong lớp lá chuối xanh biếc. Vào buổi sáng, nhiều người xếp hàng dài để mua xôi nóng hổi. Món ăn là sự kết hợp tinh tế giữa màu sắc và hương vị, được đánh giá là ngon nhất “vịnh Bắc Bộ”.</t>
+  </si>
+  <si>
+    <t>Miêu tả đầy đủ món ốc nấu chuối đậu tại Quán Ốc Dì Tú.</t>
+  </si>
+  <si>
+    <t>Tại Quán Ốc Dì Tú, món ốc nấu chuối đậu có ốc tươi rói, giòn sần sật, kết hợp với chuối đậu bùi bùi và nước dùng đậm đà. Hương vị độc đáo khiến thực khách muốn thưởng thức mãi không thôi. Đây là món ăn nổi bật và được nhiều thực khách yêu thích.</t>
+  </si>
+  <si>
+    <t>Bún ốc Hà Nội được làm từ những nguyên liệu chính nào?</t>
+  </si>
+  <si>
+    <t>Bún ốc Hà Nội được làm từ ốc nhồi hoặc ốc vặn, bún tươi, cà chua chín mọng, rau thơm và gia vị dân dã. Nước dùng được ninh từ xương và nước luộc ốc, thêm giấm bỗng tạo vị chua nhẹ đặc trưng.</t>
+  </si>
+  <si>
+    <t>Địa chỉ bán phở Gia Truyền ở Hà Nội là đâu?</t>
+  </si>
+  <si>
+    <t>Phở Gia Truyền có địa chỉ: 49 Bát Đàn, Quận Hoàn Kiếm, Hà Nội.</t>
+  </si>
+  <si>
+    <t>Miến lươn Hà Nội có những thành phần nào?</t>
+  </si>
+  <si>
+    <t>Miến lươn được làm từ miến, lươn, hành lá, tía tô, rau răm, lạc rang, cùng nước dùng có vị ngọt, vị thơm ngậy của lươn, vị cay của ớt và hương thơm từ rau thơm.</t>
+  </si>
+  <si>
+    <t>Gà luộc Hà Nội khi ăn thường chấm với gì?</t>
+  </si>
+  <si>
+    <t>Gà luộc Hà Nội thường được chấm với muối tiêu chanh hoặc mắm gừng.</t>
+  </si>
+  <si>
+    <t>Địa chỉ bán Kem Tràng Tiền: 35 Tràng Tiền, Quận Hoàn Kiếm, Hà Nội.</t>
+  </si>
+  <si>
+    <t>Địa chỉ bán Kem Tràng Tiền chỗ nào?</t>
+  </si>
+  <si>
+    <t>Hãy mô tả hương vị và thành phần của món Phở Cuốn Hà Nội.</t>
+  </si>
+  <si>
+    <t>Phở cuốn gồm những lát bánh phở mềm cuộn thịt bò xào, rau sống, giá đỗ và dưa góp. Khi ăn được chấm với nước mắm pha tỏi ớt chua ngọt. Món ăn thanh mát, nhẹ nhàng, không cầu kỳ nhưng dễ gây nghiện.</t>
+  </si>
+  <si>
+    <t>Mô tả món Bún Mọc Dọc Mùng bao gồm những gì và hương vị ra sao?</t>
+  </si>
+  <si>
+    <t>Bún mọc dọc mùng gồm viên mọc tròn thơm mùi mộc nhĩ, khoanh chân giò mềm rục, dọc mùng giòn sần sật và nước dùng trong, ngọt thanh từ xương ống ninh kỹ. Khi ăn thêm ớt cay, hành phi sẽ tạo trải nghiệm vị giác đậm chất Hà Thành, giản dị nhưng sâu sắc.</t>
+  </si>
+  <si>
+    <t>Hãy mô tả đầy đủ cách chế biến và hương vị của món Chả Cá Lã Vọng.</t>
+  </si>
+  <si>
+    <t>Chả cá Lã Vọng được làm từ cá lăng – loại cá ít xương, thịt ngọt và săn chắc. Cá được tẩm ướp gia vị đậm đà rồi chiên vàng trong chảo mỡ nóng. Khi ăn kết hợp với rau thì là, hành lá, bún tươi và mắm tôm pha. Hương vị béo, thơm, mằn mặn, dậy mùi đặc trưng, để lại dư vị khó quên.</t>
+  </si>
+  <si>
+    <t>Nêu mô tả đầy đủ về món sữa chua nếp cẩm Hà Nội.</t>
+  </si>
+  <si>
+    <t>Sữa chua nếp cẩm kết hợp vị chua dịu của sữa chua và vị ngọt bùi của nếp cẩm. Nếp có màu tím sẫm, ăn cùng sữa chua trắng mịn, thêm dừa khô và lạc rang giòn rụm. Hương vị gồm chút béo, chút thanh mát và dẻo bùi hòa quyện, là món ăn vặt quen thuộc của người Hà Nội.</t>
+  </si>
+  <si>
+    <t>bún riêu cua Hà Nội được chế biến như thế nào và có những thành phần gì?</t>
+  </si>
+  <si>
+    <t>Bún riêu cua được làm từ cua đồng tươi giã nhuyễn, lọc lấy nước rồi đun nhỏ lửa để riêu cua kết thành từng mảng mềm. Nước dùng có cà chua tạo màu, thêm mắm tôm, đậu phụ rán vàng giòn, giò lụa, hành lá và rau sống. Hương vị đậm đà, có giấm bỗng chua thanh và ớt tươi tạo phong vị “rất Hà Nội”.</t>
+  </si>
 </sst>
 </file>
 
@@ -667,7 +924,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -677,6 +934,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF535FC1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -723,7 +986,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -732,6 +995,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1016,8 +1282,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1315,18 +1581,18 @@
       </c>
     </row>
     <row r="37" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
+      <c r="A37" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="4" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="4" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1451,10 +1717,10 @@
       </c>
     </row>
     <row r="54" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
+      <c r="A54" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="4" t="s">
         <v>107</v>
       </c>
     </row>
@@ -1570,39 +1836,270 @@
         <v>135</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="81" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="82" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="83" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="84" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="85" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="86" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="87" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="88" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="89" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="90" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="91" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="92" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="93" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="94" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="95" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="96" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="49.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A78" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A82" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A85" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A89" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A93" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A94" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B94" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A95" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="B95" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="B96" s="3" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A97" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="B97" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B99" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B101" s="3" t="s">
+        <v>201</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>